<commit_message>
Update Inverter Loss Calculation.xlsx
</commit_message>
<xml_diff>
--- a/Calculations/Inverter Loss Calculation.xlsx
+++ b/Calculations/Inverter Loss Calculation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faheem/SemesterProjectPED2/Calculations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faheem/Documents/GitHub/SemesterProjectPED2/Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074F7C91-2020-1A4F-89A8-28B097B468BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{402DD9A7-DAFF-BE48-9E79-FB12B125226B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14540" activeTab="2" xr2:uid="{E68F2451-9246-4647-8054-A89E0E311DC4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="98">
   <si>
     <t>Inverter Evaluation</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>Tj = 25℃, Vsd = 0.68V → 0.9V, If = 1 → 200A</t>
+  </si>
+  <si>
+    <t>Eiss (pJ)</t>
   </si>
 </sst>
 </file>
@@ -4029,10 +4032,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B82EB2-F7B8-394C-B6A6-CA9828326101}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:G27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4042,7 +4045,7 @@
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -4053,13 +4056,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -4087,8 +4090,11 @@
       <c r="I4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13000</v>
       </c>
@@ -4121,7 +4127,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>9000</v>
       </c>
@@ -4155,7 +4161,7 @@
         <v>3.4329999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6000</v>
       </c>
@@ -4189,7 +4195,7 @@
         <v>1.56433</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3500</v>
       </c>
@@ -4223,7 +4229,7 @@
         <v>2.3833299999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2200</v>
       </c>
@@ -4257,7 +4263,7 @@
         <v>2.8915299999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2000</v>
       </c>
@@ -4291,13 +4297,13 @@
         <v>3.45153</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I14" s="4">
         <f>(A5*E5)+I13</f>
         <v>1300</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>65</v>
       </c>
@@ -4308,7 +4314,7 @@
         <v>18400</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -4535,7 +4541,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>